<commit_message>
DR : 개발가이드 reservations 예약상태 column 추가
</commit_message>
<xml_diff>
--- a/doc/A렌트카_개발가이드1.0.xlsx
+++ b/doc/A렌트카_개발가이드1.0.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11595" firstSheet="4" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11595" firstSheet="4" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="개발환경" sheetId="5" r:id="rId1"/>
@@ -35,7 +35,7 @@
     <sheet name="요구사항정의서" sheetId="37" r:id="rId21"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'테이블 컬럼명'!$A$1:$M$80</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'테이블 컬럼명'!$A$1:$M$81</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2408" uniqueCount="1398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2422" uniqueCount="1404">
   <si>
     <t>개발환경</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -14206,6 +14206,30 @@
   </si>
   <si>
     <t>insurance_type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>예약상태</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reservation_status</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>char</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>not null</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>no</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -14612,11 +14636,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -15105,10 +15129,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I86"/>
+  <dimension ref="A1:I87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="A87" sqref="A87:XFD87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -17174,6 +17198,32 @@
       </c>
       <c r="H86" s="12" t="s">
         <v>1395</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A87" s="12" t="s">
+        <v>1398</v>
+      </c>
+      <c r="B87" s="12" t="s">
+        <v>1399</v>
+      </c>
+      <c r="C87" s="12" t="s">
+        <v>1400</v>
+      </c>
+      <c r="D87">
+        <v>1</v>
+      </c>
+      <c r="E87" s="12" t="s">
+        <v>1401</v>
+      </c>
+      <c r="F87">
+        <v>1</v>
+      </c>
+      <c r="G87" s="12" t="s">
+        <v>1402</v>
+      </c>
+      <c r="H87" s="12" t="s">
+        <v>1403</v>
       </c>
     </row>
   </sheetData>
@@ -22536,10 +22586,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="41" t="s">
         <v>1390</v>
       </c>
-      <c r="B1" s="40"/>
+      <c r="B1" s="41"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="23" t="s">
@@ -22590,7 +22640,7 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="41" t="s">
+      <c r="A8" s="40" t="s">
         <v>1362</v>
       </c>
       <c r="B8" s="20" t="s">
@@ -22598,25 +22648,25 @@
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="41"/>
+      <c r="A9" s="40"/>
       <c r="B9" s="20" t="s">
         <v>1364</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="41"/>
+      <c r="A10" s="40"/>
       <c r="B10" s="20" t="s">
         <v>1365</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="41"/>
+      <c r="A11" s="40"/>
       <c r="B11" s="20" t="s">
         <v>1366</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="41" t="s">
+      <c r="A12" s="40" t="s">
         <v>1367</v>
       </c>
       <c r="B12" s="24" t="s">
@@ -22624,25 +22674,25 @@
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="41"/>
+      <c r="A13" s="40"/>
       <c r="B13" s="20" t="s">
         <v>1369</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="41"/>
+      <c r="A14" s="40"/>
       <c r="B14" s="24" t="s">
         <v>1370</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="41"/>
+      <c r="A15" s="40"/>
       <c r="B15" s="20" t="s">
         <v>1371</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="41" t="s">
+      <c r="A16" s="40" t="s">
         <v>1372</v>
       </c>
       <c r="B16" s="24" t="s">
@@ -22650,37 +22700,37 @@
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="41"/>
+      <c r="A17" s="40"/>
       <c r="B17" s="20" t="s">
         <v>1374</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="41"/>
+      <c r="A18" s="40"/>
       <c r="B18" s="24" t="s">
         <v>1375</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="41"/>
+      <c r="A19" s="40"/>
       <c r="B19" s="20" t="s">
         <v>1376</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="41"/>
+      <c r="A20" s="40"/>
       <c r="B20" s="24" t="s">
         <v>1377</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="41"/>
+      <c r="A21" s="40"/>
       <c r="B21" s="20" t="s">
         <v>1378</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="41" t="s">
+      <c r="A22" s="40" t="s">
         <v>1379</v>
       </c>
       <c r="B22" s="20" t="s">
@@ -22688,13 +22738,13 @@
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="41"/>
+      <c r="A23" s="40"/>
       <c r="B23" s="20" t="s">
         <v>1381</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="41" t="s">
+      <c r="A24" s="40" t="s">
         <v>1382</v>
       </c>
       <c r="B24" s="20" t="s">
@@ -22702,13 +22752,13 @@
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="41"/>
+      <c r="A25" s="40"/>
       <c r="B25" s="20" t="s">
         <v>1384</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="41" t="s">
+      <c r="A26" s="40" t="s">
         <v>1385</v>
       </c>
       <c r="B26" s="20" t="s">
@@ -22716,7 +22766,7 @@
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="41"/>
+      <c r="A27" s="40"/>
       <c r="B27" s="20" t="s">
         <v>1387</v>
       </c>
@@ -25910,10 +25960,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M122"/>
+  <dimension ref="A1:M123"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -28098,7 +28148,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="58" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>1179</v>
       </c>
@@ -28106,31 +28156,29 @@
         <v>1186</v>
       </c>
       <c r="C58" s="12" t="s">
-        <v>915</v>
-      </c>
-      <c r="D58" t="str">
-        <f>VLOOKUP(C58,컬럼명!$A$2:$H$179,2,FALSE)</f>
-        <v>created_at</v>
-      </c>
-      <c r="E58" t="str">
-        <f>VLOOKUP(C58,컬럼명!$A$2:$H$179,3,FALSE)</f>
-        <v>timestamp</v>
-      </c>
-      <c r="F58" t="str">
-        <f>VLOOKUP(C58,컬럼명!$A$2:$H$179,4,FALSE)</f>
-        <v/>
-      </c>
-      <c r="G58"/>
-      <c r="H58"/>
-      <c r="I58" t="str">
-        <f>VLOOKUP(C58,컬럼명!$A$2:$H$179,7,FALSE)</f>
-        <v>sysdate</v>
-      </c>
-      <c r="J58" t="str">
-        <f>VLOOKUP(C58,컬럼명!$A$2:$H$179,8,FALSE)</f>
-        <v>create</v>
-      </c>
-      <c r="K58"/>
+        <v>1398</v>
+      </c>
+      <c r="D58" s="12" t="s">
+        <v>1399</v>
+      </c>
+      <c r="E58" s="12" t="s">
+        <v>1400</v>
+      </c>
+      <c r="F58">
+        <v>1</v>
+      </c>
+      <c r="G58" s="12" t="s">
+        <v>1401</v>
+      </c>
+      <c r="H58">
+        <v>1</v>
+      </c>
+      <c r="I58" s="12" t="s">
+        <v>1402</v>
+      </c>
+      <c r="J58" s="12" t="s">
+        <v>1403</v>
+      </c>
       <c r="L58">
         <v>14</v>
       </c>
@@ -28143,11 +28191,11 @@
         <v>1186</v>
       </c>
       <c r="C59" s="12" t="s">
-        <v>910</v>
+        <v>915</v>
       </c>
       <c r="D59" t="str">
         <f>VLOOKUP(C59,컬럼명!$A$2:$H$179,2,FALSE)</f>
-        <v>updated_at</v>
+        <v>created_at</v>
       </c>
       <c r="E59" t="str">
         <f>VLOOKUP(C59,컬럼명!$A$2:$H$179,3,FALSE)</f>
@@ -28165,55 +28213,48 @@
       </c>
       <c r="J59" t="str">
         <f>VLOOKUP(C59,컬럼명!$A$2:$H$179,8,FALSE)</f>
-        <v>update</v>
+        <v>create</v>
       </c>
       <c r="K59"/>
       <c r="L59">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="B60" t="s">
-        <v>1064</v>
-      </c>
-      <c r="C60" t="s">
-        <v>1109</v>
+        <v>1186</v>
+      </c>
+      <c r="C60" s="12" t="s">
+        <v>910</v>
       </c>
       <c r="D60" t="str">
         <f>VLOOKUP(C60,컬럼명!$A$2:$H$179,2,FALSE)</f>
-        <v>user_code</v>
+        <v>updated_at</v>
       </c>
       <c r="E60" t="str">
         <f>VLOOKUP(C60,컬럼명!$A$2:$H$179,3,FALSE)</f>
-        <v>int</v>
+        <v>timestamp</v>
       </c>
       <c r="F60" t="str">
         <f>VLOOKUP(C60,컬럼명!$A$2:$H$179,4,FALSE)</f>
         <v/>
       </c>
-      <c r="G60" t="str">
-        <f>VLOOKUP(C60,컬럼명!$A$2:$H$179,5,FALSE)</f>
-        <v>not null</v>
-      </c>
+      <c r="G60"/>
+      <c r="H60"/>
       <c r="I60" t="str">
         <f>VLOOKUP(C60,컬럼명!$A$2:$H$179,7,FALSE)</f>
-        <v>code</v>
+        <v>sysdate</v>
       </c>
       <c r="J60" t="str">
         <f>VLOOKUP(C60,컬럼명!$A$2:$H$179,8,FALSE)</f>
-        <v>no</v>
-      </c>
-      <c r="K60">
-        <v>1</v>
-      </c>
+        <v>update</v>
+      </c>
+      <c r="K60"/>
       <c r="L60">
-        <v>1</v>
-      </c>
-      <c r="M60">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.3">
@@ -28223,20 +28264,20 @@
       <c r="B61" t="s">
         <v>1064</v>
       </c>
-      <c r="C61" s="12" t="s">
-        <v>901</v>
+      <c r="C61" t="s">
+        <v>1109</v>
       </c>
       <c r="D61" t="str">
         <f>VLOOKUP(C61,컬럼명!$A$2:$H$179,2,FALSE)</f>
-        <v>user_email</v>
+        <v>user_code</v>
       </c>
       <c r="E61" t="str">
         <f>VLOOKUP(C61,컬럼명!$A$2:$H$179,3,FALSE)</f>
-        <v>varchar</v>
-      </c>
-      <c r="F61">
+        <v>int</v>
+      </c>
+      <c r="F61" t="str">
         <f>VLOOKUP(C61,컬럼명!$A$2:$H$179,4,FALSE)</f>
-        <v>100</v>
+        <v/>
       </c>
       <c r="G61" t="str">
         <f>VLOOKUP(C61,컬럼명!$A$2:$H$179,5,FALSE)</f>
@@ -28244,14 +28285,20 @@
       </c>
       <c r="I61" t="str">
         <f>VLOOKUP(C61,컬럼명!$A$2:$H$179,7,FALSE)</f>
-        <v>name</v>
+        <v>code</v>
       </c>
       <c r="J61" t="str">
         <f>VLOOKUP(C61,컬럼명!$A$2:$H$179,8,FALSE)</f>
         <v>no</v>
       </c>
+      <c r="K61">
+        <v>1</v>
+      </c>
       <c r="L61">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="M61">
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.3">
@@ -28262,11 +28309,11 @@
         <v>1064</v>
       </c>
       <c r="C62" s="12" t="s">
-        <v>229</v>
+        <v>901</v>
       </c>
       <c r="D62" t="str">
         <f>VLOOKUP(C62,컬럼명!$A$2:$H$179,2,FALSE)</f>
-        <v>user_name</v>
+        <v>user_email</v>
       </c>
       <c r="E62" t="str">
         <f>VLOOKUP(C62,컬럼명!$A$2:$H$179,3,FALSE)</f>
@@ -28289,7 +28336,7 @@
         <v>no</v>
       </c>
       <c r="L62">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.3">
@@ -28300,11 +28347,11 @@
         <v>1064</v>
       </c>
       <c r="C63" s="12" t="s">
-        <v>907</v>
+        <v>229</v>
       </c>
       <c r="D63" t="str">
         <f>VLOOKUP(C63,컬럼명!$A$2:$H$179,2,FALSE)</f>
-        <v>user_password</v>
+        <v>user_name</v>
       </c>
       <c r="E63" t="str">
         <f>VLOOKUP(C63,컬럼명!$A$2:$H$179,3,FALSE)</f>
@@ -28327,7 +28374,7 @@
         <v>no</v>
       </c>
       <c r="L63">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.3">
@@ -28338,11 +28385,11 @@
         <v>1064</v>
       </c>
       <c r="C64" s="12" t="s">
-        <v>905</v>
+        <v>907</v>
       </c>
       <c r="D64" t="str">
         <f>VLOOKUP(C64,컬럼명!$A$2:$H$179,2,FALSE)</f>
-        <v>user_phone_number</v>
+        <v>user_password</v>
       </c>
       <c r="E64" t="str">
         <f>VLOOKUP(C64,컬럼명!$A$2:$H$179,3,FALSE)</f>
@@ -28350,7 +28397,7 @@
       </c>
       <c r="F64">
         <f>VLOOKUP(C64,컬럼명!$A$2:$H$179,4,FALSE)</f>
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="G64" t="str">
         <f>VLOOKUP(C64,컬럼명!$A$2:$H$179,5,FALSE)</f>
@@ -28365,7 +28412,7 @@
         <v>no</v>
       </c>
       <c r="L64">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.3">
@@ -28376,19 +28423,19 @@
         <v>1064</v>
       </c>
       <c r="C65" s="12" t="s">
-        <v>1063</v>
+        <v>905</v>
       </c>
       <c r="D65" t="str">
         <f>VLOOKUP(C65,컬럼명!$A$2:$H$179,2,FALSE)</f>
-        <v>user_birth_date</v>
+        <v>user_phone_number</v>
       </c>
       <c r="E65" t="str">
         <f>VLOOKUP(C65,컬럼명!$A$2:$H$179,3,FALSE)</f>
-        <v>char</v>
+        <v>varchar</v>
       </c>
       <c r="F65">
         <f>VLOOKUP(C65,컬럼명!$A$2:$H$179,4,FALSE)</f>
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="G65" t="str">
         <f>VLOOKUP(C65,컬럼명!$A$2:$H$179,5,FALSE)</f>
@@ -28396,14 +28443,14 @@
       </c>
       <c r="I65" t="str">
         <f>VLOOKUP(C65,컬럼명!$A$2:$H$179,7,FALSE)</f>
-        <v>date</v>
+        <v>name</v>
       </c>
       <c r="J65" t="str">
         <f>VLOOKUP(C65,컬럼명!$A$2:$H$179,8,FALSE)</f>
         <v>no</v>
       </c>
       <c r="L65">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.3">
@@ -28413,20 +28460,20 @@
       <c r="B66" t="s">
         <v>1064</v>
       </c>
-      <c r="C66" t="s">
-        <v>1094</v>
+      <c r="C66" s="12" t="s">
+        <v>1063</v>
       </c>
       <c r="D66" t="str">
         <f>VLOOKUP(C66,컬럼명!$A$2:$H$179,2,FALSE)</f>
-        <v>driver_license_number</v>
+        <v>user_birth_date</v>
       </c>
       <c r="E66" t="str">
         <f>VLOOKUP(C66,컬럼명!$A$2:$H$179,3,FALSE)</f>
-        <v>varchar</v>
+        <v>char</v>
       </c>
       <c r="F66">
         <f>VLOOKUP(C66,컬럼명!$A$2:$H$179,4,FALSE)</f>
-        <v>50</v>
+        <v>8</v>
       </c>
       <c r="G66" t="str">
         <f>VLOOKUP(C66,컬럼명!$A$2:$H$179,5,FALSE)</f>
@@ -28434,14 +28481,14 @@
       </c>
       <c r="I66" t="str">
         <f>VLOOKUP(C66,컬럼명!$A$2:$H$179,7,FALSE)</f>
-        <v>name</v>
+        <v>date</v>
       </c>
       <c r="J66" t="str">
         <f>VLOOKUP(C66,컬럼명!$A$2:$H$179,8,FALSE)</f>
         <v>no</v>
       </c>
       <c r="L66">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.3">
@@ -28452,19 +28499,19 @@
         <v>1064</v>
       </c>
       <c r="C67" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="D67" t="str">
         <f>VLOOKUP(C67,컬럼명!$A$2:$H$179,2,FALSE)</f>
-        <v>license_expiry_date</v>
+        <v>driver_license_number</v>
       </c>
       <c r="E67" t="str">
         <f>VLOOKUP(C67,컬럼명!$A$2:$H$179,3,FALSE)</f>
-        <v>char</v>
+        <v>varchar</v>
       </c>
       <c r="F67">
         <f>VLOOKUP(C67,컬럼명!$A$2:$H$179,4,FALSE)</f>
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="G67" t="str">
         <f>VLOOKUP(C67,컬럼명!$A$2:$H$179,5,FALSE)</f>
@@ -28472,14 +28519,14 @@
       </c>
       <c r="I67" t="str">
         <f>VLOOKUP(C67,컬럼명!$A$2:$H$179,7,FALSE)</f>
-        <v>date</v>
+        <v>name</v>
       </c>
       <c r="J67" t="str">
         <f>VLOOKUP(C67,컬럼명!$A$2:$H$179,8,FALSE)</f>
         <v>no</v>
       </c>
       <c r="L67">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.3">
@@ -28490,11 +28537,11 @@
         <v>1064</v>
       </c>
       <c r="C68" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="D68" t="str">
         <f>VLOOKUP(C68,컬럼명!$A$2:$H$179,2,FALSE)</f>
-        <v>license_issue_date</v>
+        <v>license_expiry_date</v>
       </c>
       <c r="E68" t="str">
         <f>VLOOKUP(C68,컬럼명!$A$2:$H$179,3,FALSE)</f>
@@ -28517,7 +28564,7 @@
         <v>no</v>
       </c>
       <c r="L68">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.3">
@@ -28527,12 +28574,12 @@
       <c r="B69" t="s">
         <v>1064</v>
       </c>
-      <c r="C69" s="12" t="s">
-        <v>230</v>
+      <c r="C69" t="s">
+        <v>1096</v>
       </c>
       <c r="D69" t="str">
         <f>VLOOKUP(C69,컬럼명!$A$2:$H$179,2,FALSE)</f>
-        <v>user_category</v>
+        <v>license_issue_date</v>
       </c>
       <c r="E69" t="str">
         <f>VLOOKUP(C69,컬럼명!$A$2:$H$179,3,FALSE)</f>
@@ -28540,7 +28587,7 @@
       </c>
       <c r="F69">
         <f>VLOOKUP(C69,컬럼명!$A$2:$H$179,4,FALSE)</f>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G69" t="str">
         <f>VLOOKUP(C69,컬럼명!$A$2:$H$179,5,FALSE)</f>
@@ -28548,14 +28595,14 @@
       </c>
       <c r="I69" t="str">
         <f>VLOOKUP(C69,컬럼명!$A$2:$H$179,7,FALSE)</f>
-        <v>name</v>
+        <v>date</v>
       </c>
       <c r="J69" t="str">
         <f>VLOOKUP(C69,컬럼명!$A$2:$H$179,8,FALSE)</f>
         <v>no</v>
       </c>
       <c r="L69">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.3">
@@ -28566,11 +28613,11 @@
         <v>1064</v>
       </c>
       <c r="C70" s="12" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D70" t="str">
         <f>VLOOKUP(C70,컬럼명!$A$2:$H$179,2,FALSE)</f>
-        <v>usage_status</v>
+        <v>user_category</v>
       </c>
       <c r="E70" t="str">
         <f>VLOOKUP(C70,컬럼명!$A$2:$H$179,3,FALSE)</f>
@@ -28593,10 +28640,10 @@
         <v>no</v>
       </c>
       <c r="L70">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="71" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>1180</v>
       </c>
@@ -28604,33 +28651,34 @@
         <v>1064</v>
       </c>
       <c r="C71" s="12" t="s">
-        <v>915</v>
+        <v>231</v>
       </c>
       <c r="D71" t="str">
         <f>VLOOKUP(C71,컬럼명!$A$2:$H$179,2,FALSE)</f>
-        <v>created_at</v>
+        <v>usage_status</v>
       </c>
       <c r="E71" t="str">
         <f>VLOOKUP(C71,컬럼명!$A$2:$H$179,3,FALSE)</f>
-        <v>timestamp</v>
-      </c>
-      <c r="F71" t="str">
+        <v>char</v>
+      </c>
+      <c r="F71">
         <f>VLOOKUP(C71,컬럼명!$A$2:$H$179,4,FALSE)</f>
-        <v/>
-      </c>
-      <c r="G71"/>
-      <c r="H71"/>
+        <v>1</v>
+      </c>
+      <c r="G71" t="str">
+        <f>VLOOKUP(C71,컬럼명!$A$2:$H$179,5,FALSE)</f>
+        <v>not null</v>
+      </c>
       <c r="I71" t="str">
         <f>VLOOKUP(C71,컬럼명!$A$2:$H$179,7,FALSE)</f>
-        <v>sysdate</v>
+        <v>name</v>
       </c>
       <c r="J71" t="str">
         <f>VLOOKUP(C71,컬럼명!$A$2:$H$179,8,FALSE)</f>
-        <v>create</v>
-      </c>
-      <c r="K71"/>
+        <v>no</v>
+      </c>
       <c r="L71">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="72" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -28641,11 +28689,11 @@
         <v>1064</v>
       </c>
       <c r="C72" s="12" t="s">
-        <v>910</v>
+        <v>915</v>
       </c>
       <c r="D72" t="str">
         <f>VLOOKUP(C72,컬럼명!$A$2:$H$179,2,FALSE)</f>
-        <v>updated_at</v>
+        <v>created_at</v>
       </c>
       <c r="E72" t="str">
         <f>VLOOKUP(C72,컬럼명!$A$2:$H$179,3,FALSE)</f>
@@ -28663,55 +28711,48 @@
       </c>
       <c r="J72" t="str">
         <f>VLOOKUP(C72,컬럼명!$A$2:$H$179,8,FALSE)</f>
-        <v>update</v>
+        <v>create</v>
       </c>
       <c r="K72"/>
       <c r="L72">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="B73" t="s">
-        <v>1236</v>
-      </c>
-      <c r="C73" t="s">
-        <v>1111</v>
+        <v>1064</v>
+      </c>
+      <c r="C73" s="12" t="s">
+        <v>910</v>
       </c>
       <c r="D73" t="str">
         <f>VLOOKUP(C73,컬럼명!$A$2:$H$179,2,FALSE)</f>
-        <v>admin_code</v>
+        <v>updated_at</v>
       </c>
       <c r="E73" t="str">
         <f>VLOOKUP(C73,컬럼명!$A$2:$H$179,3,FALSE)</f>
-        <v>int</v>
+        <v>timestamp</v>
       </c>
       <c r="F73" t="str">
         <f>VLOOKUP(C73,컬럼명!$A$2:$H$179,4,FALSE)</f>
         <v/>
       </c>
-      <c r="G73" t="str">
-        <f>VLOOKUP(C73,컬럼명!$A$2:$H$179,5,FALSE)</f>
-        <v>not null</v>
-      </c>
+      <c r="G73"/>
+      <c r="H73"/>
       <c r="I73" t="str">
         <f>VLOOKUP(C73,컬럼명!$A$2:$H$179,7,FALSE)</f>
-        <v>code</v>
+        <v>sysdate</v>
       </c>
       <c r="J73" t="str">
         <f>VLOOKUP(C73,컬럼명!$A$2:$H$179,8,FALSE)</f>
-        <v>no</v>
-      </c>
-      <c r="K73">
-        <v>1</v>
-      </c>
+        <v>update</v>
+      </c>
+      <c r="K73"/>
       <c r="L73">
-        <v>1</v>
-      </c>
-      <c r="M73">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.3">
@@ -28722,19 +28763,19 @@
         <v>1236</v>
       </c>
       <c r="C74" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="D74" t="str">
         <f>VLOOKUP(C74,컬럼명!$A$2:$H$179,2,FALSE)</f>
-        <v>admin_id</v>
+        <v>admin_code</v>
       </c>
       <c r="E74" t="str">
         <f>VLOOKUP(C74,컬럼명!$A$2:$H$179,3,FALSE)</f>
-        <v>varchar</v>
-      </c>
-      <c r="F74">
+        <v>int</v>
+      </c>
+      <c r="F74" t="str">
         <f>VLOOKUP(C74,컬럼명!$A$2:$H$179,4,FALSE)</f>
-        <v>50</v>
+        <v/>
       </c>
       <c r="G74" t="str">
         <f>VLOOKUP(C74,컬럼명!$A$2:$H$179,5,FALSE)</f>
@@ -28742,14 +28783,20 @@
       </c>
       <c r="I74" t="str">
         <f>VLOOKUP(C74,컬럼명!$A$2:$H$179,7,FALSE)</f>
-        <v>name</v>
+        <v>code</v>
       </c>
       <c r="J74" t="str">
         <f>VLOOKUP(C74,컬럼명!$A$2:$H$179,8,FALSE)</f>
         <v>no</v>
       </c>
+      <c r="K74">
+        <v>1</v>
+      </c>
       <c r="L74">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="M74">
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.3">
@@ -28760,11 +28807,11 @@
         <v>1236</v>
       </c>
       <c r="C75" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="D75" t="str">
         <f>VLOOKUP(C75,컬럼명!$A$2:$H$179,2,FALSE)</f>
-        <v>admin_password</v>
+        <v>admin_id</v>
       </c>
       <c r="E75" t="str">
         <f>VLOOKUP(C75,컬럼명!$A$2:$H$179,3,FALSE)</f>
@@ -28772,7 +28819,7 @@
       </c>
       <c r="F75">
         <f>VLOOKUP(C75,컬럼명!$A$2:$H$179,4,FALSE)</f>
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="G75" t="str">
         <f>VLOOKUP(C75,컬럼명!$A$2:$H$179,5,FALSE)</f>
@@ -28787,7 +28834,7 @@
         <v>no</v>
       </c>
       <c r="L75">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.3">
@@ -28798,11 +28845,11 @@
         <v>1236</v>
       </c>
       <c r="C76" t="s">
-        <v>1120</v>
+        <v>1113</v>
       </c>
       <c r="D76" t="str">
         <f>VLOOKUP(C76,컬럼명!$A$2:$H$179,2,FALSE)</f>
-        <v>admin_name</v>
+        <v>admin_password</v>
       </c>
       <c r="E76" t="str">
         <f>VLOOKUP(C76,컬럼명!$A$2:$H$179,3,FALSE)</f>
@@ -28825,7 +28872,7 @@
         <v>no</v>
       </c>
       <c r="L76">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.3">
@@ -28836,11 +28883,11 @@
         <v>1236</v>
       </c>
       <c r="C77" t="s">
-        <v>1114</v>
+        <v>1120</v>
       </c>
       <c r="D77" t="str">
         <f>VLOOKUP(C77,컬럼명!$A$2:$H$179,2,FALSE)</f>
-        <v>admin_privileges</v>
+        <v>admin_name</v>
       </c>
       <c r="E77" t="str">
         <f>VLOOKUP(C77,컬럼명!$A$2:$H$179,3,FALSE)</f>
@@ -28848,7 +28895,7 @@
       </c>
       <c r="F77">
         <f>VLOOKUP(C77,컬럼명!$A$2:$H$179,4,FALSE)</f>
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="G77" t="str">
         <f>VLOOKUP(C77,컬럼명!$A$2:$H$179,5,FALSE)</f>
@@ -28863,7 +28910,7 @@
         <v>no</v>
       </c>
       <c r="L77">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.3">
@@ -28874,19 +28921,19 @@
         <v>1236</v>
       </c>
       <c r="C78" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="D78" t="str">
         <f>VLOOKUP(C78,컬럼명!$A$2:$H$179,2,FALSE)</f>
-        <v>usage_status</v>
+        <v>admin_privileges</v>
       </c>
       <c r="E78" t="str">
         <f>VLOOKUP(C78,컬럼명!$A$2:$H$179,3,FALSE)</f>
-        <v>char</v>
+        <v>varchar</v>
       </c>
       <c r="F78">
         <f>VLOOKUP(C78,컬럼명!$A$2:$H$179,4,FALSE)</f>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G78" t="str">
         <f>VLOOKUP(C78,컬럼명!$A$2:$H$179,5,FALSE)</f>
@@ -28901,44 +28948,45 @@
         <v>no</v>
       </c>
       <c r="L78">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="79" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>1181</v>
       </c>
       <c r="B79" t="s">
         <v>1236</v>
       </c>
-      <c r="C79" s="12" t="s">
-        <v>915</v>
+      <c r="C79" t="s">
+        <v>1115</v>
       </c>
       <c r="D79" t="str">
         <f>VLOOKUP(C79,컬럼명!$A$2:$H$179,2,FALSE)</f>
-        <v>created_at</v>
+        <v>usage_status</v>
       </c>
       <c r="E79" t="str">
         <f>VLOOKUP(C79,컬럼명!$A$2:$H$179,3,FALSE)</f>
-        <v>timestamp</v>
-      </c>
-      <c r="F79" t="str">
+        <v>char</v>
+      </c>
+      <c r="F79">
         <f>VLOOKUP(C79,컬럼명!$A$2:$H$179,4,FALSE)</f>
-        <v/>
-      </c>
-      <c r="G79"/>
-      <c r="H79"/>
+        <v>1</v>
+      </c>
+      <c r="G79" t="str">
+        <f>VLOOKUP(C79,컬럼명!$A$2:$H$179,5,FALSE)</f>
+        <v>not null</v>
+      </c>
       <c r="I79" t="str">
         <f>VLOOKUP(C79,컬럼명!$A$2:$H$179,7,FALSE)</f>
-        <v>sysdate</v>
+        <v>name</v>
       </c>
       <c r="J79" t="str">
         <f>VLOOKUP(C79,컬럼명!$A$2:$H$179,8,FALSE)</f>
-        <v>create</v>
-      </c>
-      <c r="K79"/>
+        <v>no</v>
+      </c>
       <c r="L79">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="80" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -28949,11 +28997,11 @@
         <v>1236</v>
       </c>
       <c r="C80" s="12" t="s">
-        <v>910</v>
+        <v>915</v>
       </c>
       <c r="D80" t="str">
         <f>VLOOKUP(C80,컬럼명!$A$2:$H$179,2,FALSE)</f>
-        <v>updated_at</v>
+        <v>created_at</v>
       </c>
       <c r="E80" t="str">
         <f>VLOOKUP(C80,컬럼명!$A$2:$H$179,3,FALSE)</f>
@@ -28971,55 +29019,48 @@
       </c>
       <c r="J80" t="str">
         <f>VLOOKUP(C80,컬럼명!$A$2:$H$179,8,FALSE)</f>
-        <v>update</v>
+        <v>create</v>
       </c>
       <c r="K80"/>
       <c r="L80">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A81" s="12" t="s">
-        <v>236</v>
-      </c>
-      <c r="B81" s="12" t="s">
-        <v>923</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>1181</v>
+      </c>
+      <c r="B81" t="s">
+        <v>1236</v>
       </c>
       <c r="C81" s="12" t="s">
-        <v>232</v>
+        <v>910</v>
       </c>
       <c r="D81" t="str">
         <f>VLOOKUP(C81,컬럼명!$A$2:$H$179,2,FALSE)</f>
-        <v>menu_code</v>
+        <v>updated_at</v>
       </c>
       <c r="E81" t="str">
         <f>VLOOKUP(C81,컬럼명!$A$2:$H$179,3,FALSE)</f>
-        <v>int</v>
+        <v>timestamp</v>
       </c>
       <c r="F81" t="str">
         <f>VLOOKUP(C81,컬럼명!$A$2:$H$179,4,FALSE)</f>
         <v/>
       </c>
-      <c r="G81" t="str">
-        <f>VLOOKUP(C81,컬럼명!$A$2:$H$179,5,FALSE)</f>
-        <v>not null</v>
-      </c>
+      <c r="G81"/>
+      <c r="H81"/>
       <c r="I81" t="str">
         <f>VLOOKUP(C81,컬럼명!$A$2:$H$179,7,FALSE)</f>
-        <v>code</v>
+        <v>sysdate</v>
       </c>
       <c r="J81" t="str">
         <f>VLOOKUP(C81,컬럼명!$A$2:$H$179,8,FALSE)</f>
-        <v>no</v>
-      </c>
-      <c r="K81">
-        <v>1</v>
-      </c>
+        <v>update</v>
+      </c>
+      <c r="K81"/>
       <c r="L81">
-        <v>1</v>
-      </c>
-      <c r="M81">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.3">
@@ -29030,19 +29071,19 @@
         <v>923</v>
       </c>
       <c r="C82" s="12" t="s">
-        <v>924</v>
+        <v>232</v>
       </c>
       <c r="D82" t="str">
         <f>VLOOKUP(C82,컬럼명!$A$2:$H$179,2,FALSE)</f>
-        <v>menu_kind</v>
+        <v>menu_code</v>
       </c>
       <c r="E82" t="str">
         <f>VLOOKUP(C82,컬럼명!$A$2:$H$179,3,FALSE)</f>
-        <v>char</v>
-      </c>
-      <c r="F82">
+        <v>int</v>
+      </c>
+      <c r="F82" t="str">
         <f>VLOOKUP(C82,컬럼명!$A$2:$H$179,4,FALSE)</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="G82" t="str">
         <f>VLOOKUP(C82,컬럼명!$A$2:$H$179,5,FALSE)</f>
@@ -29056,8 +29097,14 @@
         <f>VLOOKUP(C82,컬럼명!$A$2:$H$179,8,FALSE)</f>
         <v>no</v>
       </c>
+      <c r="K82">
+        <v>1</v>
+      </c>
       <c r="L82">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="M82">
+        <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.3">
@@ -29068,11 +29115,11 @@
         <v>923</v>
       </c>
       <c r="C83" s="12" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="D83" t="str">
         <f>VLOOKUP(C83,컬럼명!$A$2:$H$179,2,FALSE)</f>
-        <v>menu_main</v>
+        <v>menu_kind</v>
       </c>
       <c r="E83" t="str">
         <f>VLOOKUP(C83,컬럼명!$A$2:$H$179,3,FALSE)</f>
@@ -29080,7 +29127,7 @@
       </c>
       <c r="F83">
         <f>VLOOKUP(C83,컬럼명!$A$2:$H$179,4,FALSE)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G83" t="str">
         <f>VLOOKUP(C83,컬럼명!$A$2:$H$179,5,FALSE)</f>
@@ -29095,7 +29142,7 @@
         <v>no</v>
       </c>
       <c r="L83">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.3">
@@ -29106,11 +29153,11 @@
         <v>923</v>
       </c>
       <c r="C84" s="12" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="D84" t="str">
         <f>VLOOKUP(C84,컬럼명!$A$2:$H$179,2,FALSE)</f>
-        <v>menu_sub</v>
+        <v>menu_main</v>
       </c>
       <c r="E84" t="str">
         <f>VLOOKUP(C84,컬럼명!$A$2:$H$179,3,FALSE)</f>
@@ -29133,7 +29180,7 @@
         <v>no</v>
       </c>
       <c r="L84">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.3">
@@ -29144,11 +29191,11 @@
         <v>923</v>
       </c>
       <c r="C85" s="12" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="D85" t="str">
         <f>VLOOKUP(C85,컬럼명!$A$2:$H$179,2,FALSE)</f>
-        <v>menu_small</v>
+        <v>menu_sub</v>
       </c>
       <c r="E85" t="str">
         <f>VLOOKUP(C85,컬럼명!$A$2:$H$179,3,FALSE)</f>
@@ -29171,7 +29218,7 @@
         <v>no</v>
       </c>
       <c r="L85">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.3">
@@ -29182,19 +29229,19 @@
         <v>923</v>
       </c>
       <c r="C86" s="12" t="s">
-        <v>330</v>
+        <v>927</v>
       </c>
       <c r="D86" t="str">
         <f>VLOOKUP(C86,컬럼명!$A$2:$H$179,2,FALSE)</f>
-        <v>menu_name</v>
+        <v>menu_small</v>
       </c>
       <c r="E86" t="str">
         <f>VLOOKUP(C86,컬럼명!$A$2:$H$179,3,FALSE)</f>
-        <v>varchar</v>
+        <v>char</v>
       </c>
       <c r="F86">
         <f>VLOOKUP(C86,컬럼명!$A$2:$H$179,4,FALSE)</f>
-        <v>100</v>
+        <v>2</v>
       </c>
       <c r="G86" t="str">
         <f>VLOOKUP(C86,컬럼명!$A$2:$H$179,5,FALSE)</f>
@@ -29202,14 +29249,14 @@
       </c>
       <c r="I86" t="str">
         <f>VLOOKUP(C86,컬럼명!$A$2:$H$179,7,FALSE)</f>
-        <v>name</v>
+        <v>code</v>
       </c>
       <c r="J86" t="str">
         <f>VLOOKUP(C86,컬럼명!$A$2:$H$179,8,FALSE)</f>
         <v>no</v>
       </c>
       <c r="L86">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.3">
@@ -29220,19 +29267,19 @@
         <v>923</v>
       </c>
       <c r="C87" s="12" t="s">
-        <v>929</v>
+        <v>330</v>
       </c>
       <c r="D87" t="str">
         <f>VLOOKUP(C87,컬럼명!$A$2:$H$179,2,FALSE)</f>
-        <v>menu_type</v>
+        <v>menu_name</v>
       </c>
       <c r="E87" t="str">
         <f>VLOOKUP(C87,컬럼명!$A$2:$H$179,3,FALSE)</f>
-        <v>char</v>
+        <v>varchar</v>
       </c>
       <c r="F87">
         <f>VLOOKUP(C87,컬럼명!$A$2:$H$179,4,FALSE)</f>
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G87" t="str">
         <f>VLOOKUP(C87,컬럼명!$A$2:$H$179,5,FALSE)</f>
@@ -29240,14 +29287,14 @@
       </c>
       <c r="I87" t="str">
         <f>VLOOKUP(C87,컬럼명!$A$2:$H$179,7,FALSE)</f>
-        <v>code</v>
+        <v>name</v>
       </c>
       <c r="J87" t="str">
         <f>VLOOKUP(C87,컬럼명!$A$2:$H$179,8,FALSE)</f>
         <v>no</v>
       </c>
       <c r="L87">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.3">
@@ -29258,30 +29305,34 @@
         <v>923</v>
       </c>
       <c r="C88" s="12" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="D88" t="str">
         <f>VLOOKUP(C88,컬럼명!$A$2:$H$179,2,FALSE)</f>
-        <v>menu_icon</v>
+        <v>menu_type</v>
       </c>
       <c r="E88" t="str">
         <f>VLOOKUP(C88,컬럼명!$A$2:$H$179,3,FALSE)</f>
-        <v>varchar</v>
+        <v>char</v>
       </c>
       <c r="F88">
         <f>VLOOKUP(C88,컬럼명!$A$2:$H$179,4,FALSE)</f>
-        <v>100</v>
+        <v>1</v>
+      </c>
+      <c r="G88" t="str">
+        <f>VLOOKUP(C88,컬럼명!$A$2:$H$179,5,FALSE)</f>
+        <v>not null</v>
       </c>
       <c r="I88" t="str">
         <f>VLOOKUP(C88,컬럼명!$A$2:$H$179,7,FALSE)</f>
-        <v>name</v>
+        <v>code</v>
       </c>
       <c r="J88" t="str">
         <f>VLOOKUP(C88,컬럼명!$A$2:$H$179,8,FALSE)</f>
         <v>no</v>
       </c>
       <c r="L88">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.3">
@@ -29292,11 +29343,11 @@
         <v>923</v>
       </c>
       <c r="C89" s="12" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="D89" t="str">
         <f>VLOOKUP(C89,컬럼명!$A$2:$H$179,2,FALSE)</f>
-        <v>menu_component</v>
+        <v>menu_icon</v>
       </c>
       <c r="E89" t="str">
         <f>VLOOKUP(C89,컬럼명!$A$2:$H$179,3,FALSE)</f>
@@ -29315,7 +29366,7 @@
         <v>no</v>
       </c>
       <c r="L89">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.3">
@@ -29326,30 +29377,30 @@
         <v>923</v>
       </c>
       <c r="C90" s="12" t="s">
-        <v>915</v>
+        <v>933</v>
       </c>
       <c r="D90" t="str">
         <f>VLOOKUP(C90,컬럼명!$A$2:$H$179,2,FALSE)</f>
-        <v>created_at</v>
+        <v>menu_component</v>
       </c>
       <c r="E90" t="str">
         <f>VLOOKUP(C90,컬럼명!$A$2:$H$179,3,FALSE)</f>
-        <v>timestamp</v>
-      </c>
-      <c r="F90" t="str">
+        <v>varchar</v>
+      </c>
+      <c r="F90">
         <f>VLOOKUP(C90,컬럼명!$A$2:$H$179,4,FALSE)</f>
-        <v/>
+        <v>100</v>
       </c>
       <c r="I90" t="str">
         <f>VLOOKUP(C90,컬럼명!$A$2:$H$179,7,FALSE)</f>
-        <v>sysdate</v>
+        <v>name</v>
       </c>
       <c r="J90" t="str">
         <f>VLOOKUP(C90,컬럼명!$A$2:$H$179,8,FALSE)</f>
-        <v>create</v>
+        <v>no</v>
       </c>
       <c r="L90">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.3">
@@ -29360,11 +29411,11 @@
         <v>923</v>
       </c>
       <c r="C91" s="12" t="s">
-        <v>910</v>
+        <v>915</v>
       </c>
       <c r="D91" t="str">
         <f>VLOOKUP(C91,컬럼명!$A$2:$H$179,2,FALSE)</f>
-        <v>updated_at</v>
+        <v>created_at</v>
       </c>
       <c r="E91" t="str">
         <f>VLOOKUP(C91,컬럼명!$A$2:$H$179,3,FALSE)</f>
@@ -29380,51 +29431,44 @@
       </c>
       <c r="J91" t="str">
         <f>VLOOKUP(C91,컬럼명!$A$2:$H$179,8,FALSE)</f>
-        <v>update</v>
+        <v>create</v>
       </c>
       <c r="L91">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A92" s="12" t="s">
-        <v>936</v>
+        <v>236</v>
       </c>
       <c r="B92" s="12" t="s">
-        <v>937</v>
+        <v>923</v>
       </c>
       <c r="C92" s="12" t="s">
-        <v>938</v>
+        <v>910</v>
       </c>
       <c r="D92" t="str">
         <f>VLOOKUP(C92,컬럼명!$A$2:$H$179,2,FALSE)</f>
-        <v>common_kind_code</v>
+        <v>updated_at</v>
       </c>
       <c r="E92" t="str">
         <f>VLOOKUP(C92,컬럼명!$A$2:$H$179,3,FALSE)</f>
-        <v>varchar</v>
-      </c>
-      <c r="F92">
+        <v>timestamp</v>
+      </c>
+      <c r="F92" t="str">
         <f>VLOOKUP(C92,컬럼명!$A$2:$H$179,4,FALSE)</f>
-        <v>20</v>
-      </c>
-      <c r="G92" t="str">
-        <f>VLOOKUP(C92,컬럼명!$A$2:$H$179,5,FALSE)</f>
-        <v>not null</v>
+        <v/>
       </c>
       <c r="I92" t="str">
         <f>VLOOKUP(C92,컬럼명!$A$2:$H$179,7,FALSE)</f>
-        <v>code</v>
+        <v>sysdate</v>
       </c>
       <c r="J92" t="str">
         <f>VLOOKUP(C92,컬럼명!$A$2:$H$179,8,FALSE)</f>
-        <v>no</v>
+        <v>update</v>
       </c>
       <c r="L92">
-        <v>1</v>
-      </c>
-      <c r="M92">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.3">
@@ -29435,11 +29479,11 @@
         <v>937</v>
       </c>
       <c r="C93" s="12" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
       <c r="D93" t="str">
         <f>VLOOKUP(C93,컬럼명!$A$2:$H$179,2,FALSE)</f>
-        <v>common_code</v>
+        <v>common_kind_code</v>
       </c>
       <c r="E93" t="str">
         <f>VLOOKUP(C93,컬럼명!$A$2:$H$179,3,FALSE)</f>
@@ -29447,7 +29491,7 @@
       </c>
       <c r="F93">
         <f>VLOOKUP(C93,컬럼명!$A$2:$H$179,4,FALSE)</f>
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="G93" t="str">
         <f>VLOOKUP(C93,컬럼명!$A$2:$H$179,5,FALSE)</f>
@@ -29462,10 +29506,10 @@
         <v>no</v>
       </c>
       <c r="L93">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M93">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.3">
@@ -29476,11 +29520,11 @@
         <v>937</v>
       </c>
       <c r="C94" s="12" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
       <c r="D94" t="str">
         <f>VLOOKUP(C94,컬럼명!$A$2:$H$179,2,FALSE)</f>
-        <v>common_name</v>
+        <v>common_code</v>
       </c>
       <c r="E94" t="str">
         <f>VLOOKUP(C94,컬럼명!$A$2:$H$179,3,FALSE)</f>
@@ -29488,7 +29532,7 @@
       </c>
       <c r="F94">
         <f>VLOOKUP(C94,컬럼명!$A$2:$H$179,4,FALSE)</f>
-        <v>200</v>
+        <v>2</v>
       </c>
       <c r="G94" t="str">
         <f>VLOOKUP(C94,컬럼명!$A$2:$H$179,5,FALSE)</f>
@@ -29496,14 +29540,17 @@
       </c>
       <c r="I94" t="str">
         <f>VLOOKUP(C94,컬럼명!$A$2:$H$179,7,FALSE)</f>
-        <v>name</v>
+        <v>code</v>
       </c>
       <c r="J94" t="str">
         <f>VLOOKUP(C94,컬럼명!$A$2:$H$179,8,FALSE)</f>
         <v>no</v>
       </c>
       <c r="L94">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="M94">
+        <v>2</v>
       </c>
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.3">
@@ -29514,30 +29561,34 @@
         <v>937</v>
       </c>
       <c r="C95" s="12" t="s">
-        <v>915</v>
+        <v>942</v>
       </c>
       <c r="D95" t="str">
         <f>VLOOKUP(C95,컬럼명!$A$2:$H$179,2,FALSE)</f>
-        <v>created_at</v>
+        <v>common_name</v>
       </c>
       <c r="E95" t="str">
         <f>VLOOKUP(C95,컬럼명!$A$2:$H$179,3,FALSE)</f>
-        <v>timestamp</v>
-      </c>
-      <c r="F95" t="str">
+        <v>varchar</v>
+      </c>
+      <c r="F95">
         <f>VLOOKUP(C95,컬럼명!$A$2:$H$179,4,FALSE)</f>
-        <v/>
+        <v>200</v>
+      </c>
+      <c r="G95" t="str">
+        <f>VLOOKUP(C95,컬럼명!$A$2:$H$179,5,FALSE)</f>
+        <v>not null</v>
       </c>
       <c r="I95" t="str">
         <f>VLOOKUP(C95,컬럼명!$A$2:$H$179,7,FALSE)</f>
-        <v>sysdate</v>
+        <v>name</v>
       </c>
       <c r="J95" t="str">
         <f>VLOOKUP(C95,컬럼명!$A$2:$H$179,8,FALSE)</f>
-        <v>create</v>
+        <v>no</v>
       </c>
       <c r="L95">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.3">
@@ -29548,11 +29599,11 @@
         <v>937</v>
       </c>
       <c r="C96" s="12" t="s">
-        <v>910</v>
+        <v>915</v>
       </c>
       <c r="D96" t="str">
         <f>VLOOKUP(C96,컬럼명!$A$2:$H$179,2,FALSE)</f>
-        <v>updated_at</v>
+        <v>created_at</v>
       </c>
       <c r="E96" t="str">
         <f>VLOOKUP(C96,컬럼명!$A$2:$H$179,3,FALSE)</f>
@@ -29568,54 +29619,44 @@
       </c>
       <c r="J96" t="str">
         <f>VLOOKUP(C96,컬럼명!$A$2:$H$179,8,FALSE)</f>
-        <v>update</v>
+        <v>create</v>
       </c>
       <c r="L96">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A97" s="12" t="s">
-        <v>1310</v>
+        <v>936</v>
       </c>
       <c r="B97" s="12" t="s">
-        <v>1311</v>
+        <v>937</v>
       </c>
       <c r="C97" s="12" t="s">
-        <v>1314</v>
+        <v>910</v>
       </c>
       <c r="D97" t="str">
         <f>VLOOKUP(C97,컬럼명!$A$2:$H$179,2,FALSE)</f>
-        <v>post_code</v>
+        <v>updated_at</v>
       </c>
       <c r="E97" t="str">
         <f>VLOOKUP(C97,컬럼명!$A$2:$H$179,3,FALSE)</f>
-        <v>int</v>
-      </c>
-      <c r="F97">
+        <v>timestamp</v>
+      </c>
+      <c r="F97" t="str">
         <f>VLOOKUP(C97,컬럼명!$A$2:$H$179,4,FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="G97" t="str">
-        <f>VLOOKUP(C97,컬럼명!$A$2:$H$179,5,FALSE)</f>
-        <v>not null</v>
+        <v/>
       </c>
       <c r="I97" t="str">
         <f>VLOOKUP(C97,컬럼명!$A$2:$H$179,7,FALSE)</f>
-        <v>code</v>
+        <v>sysdate</v>
       </c>
       <c r="J97" t="str">
         <f>VLOOKUP(C97,컬럼명!$A$2:$H$179,8,FALSE)</f>
-        <v>no</v>
-      </c>
-      <c r="K97">
-        <v>1</v>
+        <v>update</v>
       </c>
       <c r="L97">
-        <v>1</v>
-      </c>
-      <c r="M97">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.3">
@@ -29626,19 +29667,19 @@
         <v>1311</v>
       </c>
       <c r="C98" s="12" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
       <c r="D98" t="str">
         <f>VLOOKUP(C98,컬럼명!$A$2:$H$179,2,FALSE)</f>
-        <v>post_type</v>
+        <v>post_code</v>
       </c>
       <c r="E98" t="str">
         <f>VLOOKUP(C98,컬럼명!$A$2:$H$179,3,FALSE)</f>
-        <v>char</v>
+        <v>int</v>
       </c>
       <c r="F98">
         <f>VLOOKUP(C98,컬럼명!$A$2:$H$179,4,FALSE)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G98" t="str">
         <f>VLOOKUP(C98,컬럼명!$A$2:$H$179,5,FALSE)</f>
@@ -29652,8 +29693,14 @@
         <f>VLOOKUP(C98,컬럼명!$A$2:$H$179,8,FALSE)</f>
         <v>no</v>
       </c>
+      <c r="K98">
+        <v>1</v>
+      </c>
       <c r="L98">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="M98">
+        <v>1</v>
       </c>
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.3">
@@ -29664,19 +29711,19 @@
         <v>1311</v>
       </c>
       <c r="C99" s="12" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
       <c r="D99" t="str">
         <f>VLOOKUP(C99,컬럼명!$A$2:$H$179,2,FALSE)</f>
-        <v>post_title</v>
+        <v>post_type</v>
       </c>
       <c r="E99" t="str">
         <f>VLOOKUP(C99,컬럼명!$A$2:$H$179,3,FALSE)</f>
-        <v>varchar</v>
+        <v>char</v>
       </c>
       <c r="F99">
         <f>VLOOKUP(C99,컬럼명!$A$2:$H$179,4,FALSE)</f>
-        <v>100</v>
+        <v>2</v>
       </c>
       <c r="G99" t="str">
         <f>VLOOKUP(C99,컬럼명!$A$2:$H$179,5,FALSE)</f>
@@ -29684,14 +29731,14 @@
       </c>
       <c r="I99" t="str">
         <f>VLOOKUP(C99,컬럼명!$A$2:$H$179,7,FALSE)</f>
-        <v>name</v>
+        <v>code</v>
       </c>
       <c r="J99" t="str">
         <f>VLOOKUP(C99,컬럼명!$A$2:$H$179,8,FALSE)</f>
         <v>no</v>
       </c>
       <c r="L99">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.3">
@@ -29702,11 +29749,11 @@
         <v>1311</v>
       </c>
       <c r="C100" s="12" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
       <c r="D100" t="str">
         <f>VLOOKUP(C100,컬럼명!$A$2:$H$179,2,FALSE)</f>
-        <v>post_content</v>
+        <v>post_title</v>
       </c>
       <c r="E100" t="str">
         <f>VLOOKUP(C100,컬럼명!$A$2:$H$179,3,FALSE)</f>
@@ -29714,7 +29761,7 @@
       </c>
       <c r="F100">
         <f>VLOOKUP(C100,컬럼명!$A$2:$H$179,4,FALSE)</f>
-        <v>2000</v>
+        <v>100</v>
       </c>
       <c r="G100" t="str">
         <f>VLOOKUP(C100,컬럼명!$A$2:$H$179,5,FALSE)</f>
@@ -29729,7 +29776,7 @@
         <v>no</v>
       </c>
       <c r="L100">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.3">
@@ -29740,19 +29787,19 @@
         <v>1311</v>
       </c>
       <c r="C101" s="12" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
       <c r="D101" t="str">
         <f>VLOOKUP(C101,컬럼명!$A$2:$H$179,2,FALSE)</f>
-        <v>author_code</v>
+        <v>post_content</v>
       </c>
       <c r="E101" t="str">
         <f>VLOOKUP(C101,컬럼명!$A$2:$H$179,3,FALSE)</f>
-        <v>int</v>
+        <v>varchar</v>
       </c>
       <c r="F101">
         <f>VLOOKUP(C101,컬럼명!$A$2:$H$179,4,FALSE)</f>
-        <v>0</v>
+        <v>2000</v>
       </c>
       <c r="G101" t="str">
         <f>VLOOKUP(C101,컬럼명!$A$2:$H$179,5,FALSE)</f>
@@ -29767,7 +29814,7 @@
         <v>no</v>
       </c>
       <c r="L101">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.3">
@@ -29778,19 +29825,19 @@
         <v>1311</v>
       </c>
       <c r="C102" s="12" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="D102" t="str">
         <f>VLOOKUP(C102,컬럼명!$A$2:$H$179,2,FALSE)</f>
-        <v>author_tpye</v>
+        <v>author_code</v>
       </c>
       <c r="E102" t="str">
         <f>VLOOKUP(C102,컬럼명!$A$2:$H$179,3,FALSE)</f>
-        <v>char</v>
+        <v>int</v>
       </c>
       <c r="F102">
         <f>VLOOKUP(C102,컬럼명!$A$2:$H$179,4,FALSE)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G102" t="str">
         <f>VLOOKUP(C102,컬럼명!$A$2:$H$179,5,FALSE)</f>
@@ -29805,7 +29852,7 @@
         <v>no</v>
       </c>
       <c r="L102">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.3">
@@ -29816,30 +29863,34 @@
         <v>1311</v>
       </c>
       <c r="C103" s="12" t="s">
-        <v>915</v>
+        <v>1319</v>
       </c>
       <c r="D103" t="str">
         <f>VLOOKUP(C103,컬럼명!$A$2:$H$179,2,FALSE)</f>
-        <v>created_at</v>
+        <v>author_tpye</v>
       </c>
       <c r="E103" t="str">
         <f>VLOOKUP(C103,컬럼명!$A$2:$H$179,3,FALSE)</f>
-        <v>timestamp</v>
-      </c>
-      <c r="F103" t="str">
+        <v>char</v>
+      </c>
+      <c r="F103">
         <f>VLOOKUP(C103,컬럼명!$A$2:$H$179,4,FALSE)</f>
-        <v/>
+        <v>2</v>
+      </c>
+      <c r="G103" t="str">
+        <f>VLOOKUP(C103,컬럼명!$A$2:$H$179,5,FALSE)</f>
+        <v>not null</v>
       </c>
       <c r="I103" t="str">
         <f>VLOOKUP(C103,컬럼명!$A$2:$H$179,7,FALSE)</f>
-        <v>sysdate</v>
+        <v>name</v>
       </c>
       <c r="J103" t="str">
         <f>VLOOKUP(C103,컬럼명!$A$2:$H$179,8,FALSE)</f>
-        <v>create</v>
+        <v>no</v>
       </c>
       <c r="L103">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.3">
@@ -29850,11 +29901,11 @@
         <v>1311</v>
       </c>
       <c r="C104" s="12" t="s">
-        <v>910</v>
+        <v>915</v>
       </c>
       <c r="D104" t="str">
         <f>VLOOKUP(C104,컬럼명!$A$2:$H$179,2,FALSE)</f>
-        <v>updated_at</v>
+        <v>created_at</v>
       </c>
       <c r="E104" t="str">
         <f>VLOOKUP(C104,컬럼명!$A$2:$H$179,3,FALSE)</f>
@@ -29870,54 +29921,44 @@
       </c>
       <c r="J104" t="str">
         <f>VLOOKUP(C104,컬럼명!$A$2:$H$179,8,FALSE)</f>
-        <v>update</v>
+        <v>create</v>
       </c>
       <c r="L104">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A105" s="12" t="s">
-        <v>1312</v>
+        <v>1310</v>
       </c>
       <c r="B105" s="12" t="s">
-        <v>1313</v>
+        <v>1311</v>
       </c>
       <c r="C105" s="12" t="s">
-        <v>1320</v>
+        <v>910</v>
       </c>
       <c r="D105" t="str">
         <f>VLOOKUP(C105,컬럼명!$A$2:$H$179,2,FALSE)</f>
-        <v>review_code</v>
+        <v>updated_at</v>
       </c>
       <c r="E105" t="str">
         <f>VLOOKUP(C105,컬럼명!$A$2:$H$179,3,FALSE)</f>
-        <v>int</v>
-      </c>
-      <c r="F105">
+        <v>timestamp</v>
+      </c>
+      <c r="F105" t="str">
         <f>VLOOKUP(C105,컬럼명!$A$2:$H$179,4,FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="G105" t="str">
-        <f>VLOOKUP(C105,컬럼명!$A$2:$H$179,5,FALSE)</f>
-        <v>not null</v>
+        <v/>
       </c>
       <c r="I105" t="str">
         <f>VLOOKUP(C105,컬럼명!$A$2:$H$179,7,FALSE)</f>
-        <v>name</v>
+        <v>sysdate</v>
       </c>
       <c r="J105" t="str">
         <f>VLOOKUP(C105,컬럼명!$A$2:$H$179,8,FALSE)</f>
-        <v>no</v>
-      </c>
-      <c r="K105">
-        <v>1</v>
+        <v>update</v>
       </c>
       <c r="L105">
-        <v>1</v>
-      </c>
-      <c r="M105">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="106" spans="1:13" x14ac:dyDescent="0.3">
@@ -29928,11 +29969,11 @@
         <v>1313</v>
       </c>
       <c r="C106" s="12" t="s">
-        <v>1314</v>
+        <v>1320</v>
       </c>
       <c r="D106" t="str">
         <f>VLOOKUP(C106,컬럼명!$A$2:$H$179,2,FALSE)</f>
-        <v>post_code</v>
+        <v>review_code</v>
       </c>
       <c r="E106" t="str">
         <f>VLOOKUP(C106,컬럼명!$A$2:$H$179,3,FALSE)</f>
@@ -29948,14 +29989,20 @@
       </c>
       <c r="I106" t="str">
         <f>VLOOKUP(C106,컬럼명!$A$2:$H$179,7,FALSE)</f>
-        <v>code</v>
+        <v>name</v>
       </c>
       <c r="J106" t="str">
         <f>VLOOKUP(C106,컬럼명!$A$2:$H$179,8,FALSE)</f>
         <v>no</v>
       </c>
+      <c r="K106">
+        <v>1</v>
+      </c>
       <c r="L106">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="M106">
+        <v>1</v>
       </c>
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.3">
@@ -29966,11 +30013,11 @@
         <v>1313</v>
       </c>
       <c r="C107" s="12" t="s">
-        <v>1321</v>
+        <v>1314</v>
       </c>
       <c r="D107" t="str">
         <f>VLOOKUP(C107,컬럼명!$A$2:$H$179,2,FALSE)</f>
-        <v>review_rating</v>
+        <v>post_code</v>
       </c>
       <c r="E107" t="str">
         <f>VLOOKUP(C107,컬럼명!$A$2:$H$179,3,FALSE)</f>
@@ -29986,14 +30033,14 @@
       </c>
       <c r="I107" t="str">
         <f>VLOOKUP(C107,컬럼명!$A$2:$H$179,7,FALSE)</f>
-        <v>name</v>
+        <v>code</v>
       </c>
       <c r="J107" t="str">
         <f>VLOOKUP(C107,컬럼명!$A$2:$H$179,8,FALSE)</f>
         <v>no</v>
       </c>
       <c r="L107">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.3">
@@ -30004,30 +30051,34 @@
         <v>1313</v>
       </c>
       <c r="C108" s="12" t="s">
-        <v>915</v>
+        <v>1321</v>
       </c>
       <c r="D108" t="str">
         <f>VLOOKUP(C108,컬럼명!$A$2:$H$179,2,FALSE)</f>
-        <v>created_at</v>
+        <v>review_rating</v>
       </c>
       <c r="E108" t="str">
         <f>VLOOKUP(C108,컬럼명!$A$2:$H$179,3,FALSE)</f>
-        <v>timestamp</v>
-      </c>
-      <c r="F108" t="str">
+        <v>int</v>
+      </c>
+      <c r="F108">
         <f>VLOOKUP(C108,컬럼명!$A$2:$H$179,4,FALSE)</f>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="G108" t="str">
+        <f>VLOOKUP(C108,컬럼명!$A$2:$H$179,5,FALSE)</f>
+        <v>not null</v>
       </c>
       <c r="I108" t="str">
         <f>VLOOKUP(C108,컬럼명!$A$2:$H$179,7,FALSE)</f>
-        <v>sysdate</v>
+        <v>name</v>
       </c>
       <c r="J108" t="str">
         <f>VLOOKUP(C108,컬럼명!$A$2:$H$179,8,FALSE)</f>
-        <v>create</v>
+        <v>no</v>
       </c>
       <c r="L108">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.3">
@@ -30038,11 +30089,11 @@
         <v>1313</v>
       </c>
       <c r="C109" s="12" t="s">
-        <v>910</v>
+        <v>915</v>
       </c>
       <c r="D109" t="str">
         <f>VLOOKUP(C109,컬럼명!$A$2:$H$179,2,FALSE)</f>
-        <v>updated_at</v>
+        <v>created_at</v>
       </c>
       <c r="E109" t="str">
         <f>VLOOKUP(C109,컬럼명!$A$2:$H$179,3,FALSE)</f>
@@ -30058,54 +30109,44 @@
       </c>
       <c r="J109" t="str">
         <f>VLOOKUP(C109,컬럼명!$A$2:$H$179,8,FALSE)</f>
-        <v>update</v>
+        <v>create</v>
       </c>
       <c r="L109">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A110" s="12" t="s">
-        <v>1182</v>
+        <v>1312</v>
       </c>
       <c r="B110" s="12" t="s">
-        <v>1238</v>
+        <v>1313</v>
       </c>
       <c r="C110" s="12" t="s">
-        <v>1121</v>
+        <v>910</v>
       </c>
       <c r="D110" t="str">
         <f>VLOOKUP(C110,컬럼명!$A$2:$H$179,2,FALSE)</f>
-        <v>inquiry_code</v>
+        <v>updated_at</v>
       </c>
       <c r="E110" t="str">
         <f>VLOOKUP(C110,컬럼명!$A$2:$H$179,3,FALSE)</f>
-        <v>int</v>
+        <v>timestamp</v>
       </c>
       <c r="F110" t="str">
         <f>VLOOKUP(C110,컬럼명!$A$2:$H$179,4,FALSE)</f>
         <v/>
       </c>
-      <c r="G110" t="str">
-        <f>VLOOKUP(C110,컬럼명!$A$2:$H$179,5,FALSE)</f>
-        <v>not null</v>
-      </c>
       <c r="I110" t="str">
         <f>VLOOKUP(C110,컬럼명!$A$2:$H$179,7,FALSE)</f>
-        <v>code</v>
+        <v>sysdate</v>
       </c>
       <c r="J110" t="str">
         <f>VLOOKUP(C110,컬럼명!$A$2:$H$179,8,FALSE)</f>
-        <v>no</v>
-      </c>
-      <c r="K110">
-        <v>1</v>
+        <v>update</v>
       </c>
       <c r="L110">
-        <v>1</v>
-      </c>
-      <c r="M110">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.3">
@@ -30116,19 +30157,19 @@
         <v>1238</v>
       </c>
       <c r="C111" s="12" t="s">
-        <v>1314</v>
+        <v>1121</v>
       </c>
       <c r="D111" t="str">
         <f>VLOOKUP(C111,컬럼명!$A$2:$H$179,2,FALSE)</f>
-        <v>post_code</v>
+        <v>inquiry_code</v>
       </c>
       <c r="E111" t="str">
         <f>VLOOKUP(C111,컬럼명!$A$2:$H$179,3,FALSE)</f>
         <v>int</v>
       </c>
-      <c r="F111">
+      <c r="F111" t="str">
         <f>VLOOKUP(C111,컬럼명!$A$2:$H$179,4,FALSE)</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="G111" t="str">
         <f>VLOOKUP(C111,컬럼명!$A$2:$H$179,5,FALSE)</f>
@@ -30142,8 +30183,14 @@
         <f>VLOOKUP(C111,컬럼명!$A$2:$H$179,8,FALSE)</f>
         <v>no</v>
       </c>
+      <c r="K111">
+        <v>1</v>
+      </c>
       <c r="L111">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="M111">
+        <v>1</v>
       </c>
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.3">
@@ -30154,19 +30201,19 @@
         <v>1238</v>
       </c>
       <c r="C112" s="12" t="s">
-        <v>1322</v>
+        <v>1314</v>
       </c>
       <c r="D112" t="str">
         <f>VLOOKUP(C112,컬럼명!$A$2:$H$179,2,FALSE)</f>
-        <v>inquiry_status</v>
+        <v>post_code</v>
       </c>
       <c r="E112" t="str">
         <f>VLOOKUP(C112,컬럼명!$A$2:$H$179,3,FALSE)</f>
-        <v>char</v>
+        <v>int</v>
       </c>
       <c r="F112">
         <f>VLOOKUP(C112,컬럼명!$A$2:$H$179,4,FALSE)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G112" t="str">
         <f>VLOOKUP(C112,컬럼명!$A$2:$H$179,5,FALSE)</f>
@@ -30174,14 +30221,14 @@
       </c>
       <c r="I112" t="str">
         <f>VLOOKUP(C112,컬럼명!$A$2:$H$179,7,FALSE)</f>
-        <v>name</v>
+        <v>code</v>
       </c>
       <c r="J112" t="str">
         <f>VLOOKUP(C112,컬럼명!$A$2:$H$179,8,FALSE)</f>
         <v>no</v>
       </c>
       <c r="L112">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="113" spans="1:13" x14ac:dyDescent="0.3">
@@ -30192,30 +30239,34 @@
         <v>1238</v>
       </c>
       <c r="C113" s="12" t="s">
-        <v>915</v>
+        <v>1322</v>
       </c>
       <c r="D113" t="str">
         <f>VLOOKUP(C113,컬럼명!$A$2:$H$179,2,FALSE)</f>
-        <v>created_at</v>
+        <v>inquiry_status</v>
       </c>
       <c r="E113" t="str">
         <f>VLOOKUP(C113,컬럼명!$A$2:$H$179,3,FALSE)</f>
-        <v>timestamp</v>
-      </c>
-      <c r="F113" t="str">
+        <v>char</v>
+      </c>
+      <c r="F113">
         <f>VLOOKUP(C113,컬럼명!$A$2:$H$179,4,FALSE)</f>
-        <v/>
+        <v>2</v>
+      </c>
+      <c r="G113" t="str">
+        <f>VLOOKUP(C113,컬럼명!$A$2:$H$179,5,FALSE)</f>
+        <v>not null</v>
       </c>
       <c r="I113" t="str">
         <f>VLOOKUP(C113,컬럼명!$A$2:$H$179,7,FALSE)</f>
-        <v>sysdate</v>
+        <v>name</v>
       </c>
       <c r="J113" t="str">
         <f>VLOOKUP(C113,컬럼명!$A$2:$H$179,8,FALSE)</f>
-        <v>create</v>
+        <v>no</v>
       </c>
       <c r="L113">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="114" spans="1:13" x14ac:dyDescent="0.3">
@@ -30226,11 +30277,11 @@
         <v>1238</v>
       </c>
       <c r="C114" s="12" t="s">
-        <v>910</v>
+        <v>915</v>
       </c>
       <c r="D114" t="str">
         <f>VLOOKUP(C114,컬럼명!$A$2:$H$179,2,FALSE)</f>
-        <v>updated_at</v>
+        <v>created_at</v>
       </c>
       <c r="E114" t="str">
         <f>VLOOKUP(C114,컬럼명!$A$2:$H$179,3,FALSE)</f>
@@ -30246,54 +30297,44 @@
       </c>
       <c r="J114" t="str">
         <f>VLOOKUP(C114,컬럼명!$A$2:$H$179,8,FALSE)</f>
-        <v>update</v>
+        <v>create</v>
       </c>
       <c r="L114">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="115" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A115" s="12" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="B115" s="12" t="s">
-        <v>1187</v>
+        <v>1238</v>
       </c>
       <c r="C115" s="12" t="s">
-        <v>1124</v>
+        <v>910</v>
       </c>
       <c r="D115" t="str">
         <f>VLOOKUP(C115,컬럼명!$A$2:$H$179,2,FALSE)</f>
-        <v>response_code</v>
+        <v>updated_at</v>
       </c>
       <c r="E115" t="str">
         <f>VLOOKUP(C115,컬럼명!$A$2:$H$179,3,FALSE)</f>
-        <v>int</v>
+        <v>timestamp</v>
       </c>
       <c r="F115" t="str">
         <f>VLOOKUP(C115,컬럼명!$A$2:$H$179,4,FALSE)</f>
         <v/>
       </c>
-      <c r="G115" t="str">
-        <f>VLOOKUP(C115,컬럼명!$A$2:$H$179,5,FALSE)</f>
-        <v>not null</v>
-      </c>
       <c r="I115" t="str">
         <f>VLOOKUP(C115,컬럼명!$A$2:$H$179,7,FALSE)</f>
-        <v>code</v>
+        <v>sysdate</v>
       </c>
       <c r="J115" t="str">
         <f>VLOOKUP(C115,컬럼명!$A$2:$H$179,8,FALSE)</f>
-        <v>no</v>
-      </c>
-      <c r="K115">
-        <v>1</v>
+        <v>update</v>
       </c>
       <c r="L115">
-        <v>1</v>
-      </c>
-      <c r="M115">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="116" spans="1:13" x14ac:dyDescent="0.3">
@@ -30304,19 +30345,19 @@
         <v>1187</v>
       </c>
       <c r="C116" s="12" t="s">
-        <v>1314</v>
+        <v>1124</v>
       </c>
       <c r="D116" t="str">
         <f>VLOOKUP(C116,컬럼명!$A$2:$H$179,2,FALSE)</f>
-        <v>post_code</v>
+        <v>response_code</v>
       </c>
       <c r="E116" t="str">
         <f>VLOOKUP(C116,컬럼명!$A$2:$H$179,3,FALSE)</f>
         <v>int</v>
       </c>
-      <c r="F116">
+      <c r="F116" t="str">
         <f>VLOOKUP(C116,컬럼명!$A$2:$H$179,4,FALSE)</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="G116" t="str">
         <f>VLOOKUP(C116,컬럼명!$A$2:$H$179,5,FALSE)</f>
@@ -30330,8 +30371,14 @@
         <f>VLOOKUP(C116,컬럼명!$A$2:$H$179,8,FALSE)</f>
         <v>no</v>
       </c>
+      <c r="K116">
+        <v>1</v>
+      </c>
       <c r="L116">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="M116">
+        <v>1</v>
       </c>
     </row>
     <row r="117" spans="1:13" x14ac:dyDescent="0.3">
@@ -30342,19 +30389,19 @@
         <v>1187</v>
       </c>
       <c r="C117" s="12" t="s">
-        <v>1125</v>
+        <v>1314</v>
       </c>
       <c r="D117" t="str">
         <f>VLOOKUP(C117,컬럼명!$A$2:$H$179,2,FALSE)</f>
-        <v>response_content</v>
+        <v>post_code</v>
       </c>
       <c r="E117" t="str">
         <f>VLOOKUP(C117,컬럼명!$A$2:$H$179,3,FALSE)</f>
-        <v>varchar</v>
+        <v>int</v>
       </c>
       <c r="F117">
         <f>VLOOKUP(C117,컬럼명!$A$2:$H$179,4,FALSE)</f>
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="G117" t="str">
         <f>VLOOKUP(C117,컬럼명!$A$2:$H$179,5,FALSE)</f>
@@ -30362,14 +30409,14 @@
       </c>
       <c r="I117" t="str">
         <f>VLOOKUP(C117,컬럼명!$A$2:$H$179,7,FALSE)</f>
-        <v>name</v>
+        <v>code</v>
       </c>
       <c r="J117" t="str">
         <f>VLOOKUP(C117,컬럼명!$A$2:$H$179,8,FALSE)</f>
         <v>no</v>
       </c>
       <c r="L117">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="118" spans="1:13" x14ac:dyDescent="0.3">
@@ -30380,19 +30427,19 @@
         <v>1187</v>
       </c>
       <c r="C118" s="12" t="s">
-        <v>1318</v>
+        <v>1125</v>
       </c>
       <c r="D118" t="str">
         <f>VLOOKUP(C118,컬럼명!$A$2:$H$179,2,FALSE)</f>
-        <v>author_code</v>
+        <v>response_content</v>
       </c>
       <c r="E118" t="str">
         <f>VLOOKUP(C118,컬럼명!$A$2:$H$179,3,FALSE)</f>
-        <v>int</v>
+        <v>varchar</v>
       </c>
       <c r="F118">
         <f>VLOOKUP(C118,컬럼명!$A$2:$H$179,4,FALSE)</f>
-        <v>0</v>
+        <v>2000</v>
       </c>
       <c r="G118" t="str">
         <f>VLOOKUP(C118,컬럼명!$A$2:$H$179,5,FALSE)</f>
@@ -30407,7 +30454,7 @@
         <v>no</v>
       </c>
       <c r="L118">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="119" spans="1:13" x14ac:dyDescent="0.3">
@@ -30418,19 +30465,19 @@
         <v>1187</v>
       </c>
       <c r="C119" s="12" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="D119" t="str">
         <f>VLOOKUP(C119,컬럼명!$A$2:$H$179,2,FALSE)</f>
-        <v>author_tpye</v>
+        <v>author_code</v>
       </c>
       <c r="E119" t="str">
         <f>VLOOKUP(C119,컬럼명!$A$2:$H$179,3,FALSE)</f>
-        <v>char</v>
+        <v>int</v>
       </c>
       <c r="F119">
         <f>VLOOKUP(C119,컬럼명!$A$2:$H$179,4,FALSE)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G119" t="str">
         <f>VLOOKUP(C119,컬럼명!$A$2:$H$179,5,FALSE)</f>
@@ -30445,7 +30492,7 @@
         <v>no</v>
       </c>
       <c r="L119">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="120" spans="1:13" x14ac:dyDescent="0.3">
@@ -30456,30 +30503,34 @@
         <v>1187</v>
       </c>
       <c r="C120" s="12" t="s">
-        <v>915</v>
+        <v>1319</v>
       </c>
       <c r="D120" t="str">
         <f>VLOOKUP(C120,컬럼명!$A$2:$H$179,2,FALSE)</f>
-        <v>created_at</v>
+        <v>author_tpye</v>
       </c>
       <c r="E120" t="str">
         <f>VLOOKUP(C120,컬럼명!$A$2:$H$179,3,FALSE)</f>
-        <v>timestamp</v>
-      </c>
-      <c r="F120" t="str">
+        <v>char</v>
+      </c>
+      <c r="F120">
         <f>VLOOKUP(C120,컬럼명!$A$2:$H$179,4,FALSE)</f>
-        <v/>
+        <v>2</v>
+      </c>
+      <c r="G120" t="str">
+        <f>VLOOKUP(C120,컬럼명!$A$2:$H$179,5,FALSE)</f>
+        <v>not null</v>
       </c>
       <c r="I120" t="str">
         <f>VLOOKUP(C120,컬럼명!$A$2:$H$179,7,FALSE)</f>
-        <v>sysdate</v>
+        <v>name</v>
       </c>
       <c r="J120" t="str">
         <f>VLOOKUP(C120,컬럼명!$A$2:$H$179,8,FALSE)</f>
-        <v>create</v>
+        <v>no</v>
       </c>
       <c r="L120">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="121" spans="1:13" x14ac:dyDescent="0.3">
@@ -30490,11 +30541,11 @@
         <v>1187</v>
       </c>
       <c r="C121" s="12" t="s">
-        <v>910</v>
+        <v>915</v>
       </c>
       <c r="D121" t="str">
         <f>VLOOKUP(C121,컬럼명!$A$2:$H$179,2,FALSE)</f>
-        <v>updated_at</v>
+        <v>created_at</v>
       </c>
       <c r="E121" t="str">
         <f>VLOOKUP(C121,컬럼명!$A$2:$H$179,3,FALSE)</f>
@@ -30510,19 +30561,53 @@
       </c>
       <c r="J121" t="str">
         <f>VLOOKUP(C121,컬럼명!$A$2:$H$179,8,FALSE)</f>
+        <v>create</v>
+      </c>
+      <c r="L121">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="122" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A122" s="12" t="s">
+        <v>1183</v>
+      </c>
+      <c r="B122" s="12" t="s">
+        <v>1187</v>
+      </c>
+      <c r="C122" s="12" t="s">
+        <v>910</v>
+      </c>
+      <c r="D122" t="str">
+        <f>VLOOKUP(C122,컬럼명!$A$2:$H$179,2,FALSE)</f>
+        <v>updated_at</v>
+      </c>
+      <c r="E122" t="str">
+        <f>VLOOKUP(C122,컬럼명!$A$2:$H$179,3,FALSE)</f>
+        <v>timestamp</v>
+      </c>
+      <c r="F122" t="str">
+        <f>VLOOKUP(C122,컬럼명!$A$2:$H$179,4,FALSE)</f>
+        <v/>
+      </c>
+      <c r="I122" t="str">
+        <f>VLOOKUP(C122,컬럼명!$A$2:$H$179,7,FALSE)</f>
+        <v>sysdate</v>
+      </c>
+      <c r="J122" t="str">
+        <f>VLOOKUP(C122,컬럼명!$A$2:$H$179,8,FALSE)</f>
         <v>update</v>
       </c>
-      <c r="L121">
+      <c r="L122">
         <v>7</v>
       </c>
     </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A122" s="12"/>
-      <c r="B122" s="12"/>
-      <c r="C122" s="12"/>
+    <row r="123" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A123" s="12"/>
+      <c r="B123" s="12"/>
+      <c r="C123" s="12"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M80"/>
+  <autoFilter ref="A1:M81"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>